<commit_message>
flask has been added
</commit_message>
<xml_diff>
--- a/recognized_sets/recognized_multyclass.xlsx
+++ b/recognized_sets/recognized_multyclass.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="18">
   <si>
     <t>text</t>
   </si>
@@ -425,7 +425,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -791,6 +791,17 @@
         <v>1</v>
       </c>
     </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>